<commit_message>
Data edits for hydrogen power plant type
</commit_message>
<xml_diff>
--- a/InputData/elec/DCpUC/Decommissioning Cost per Unit Cap.xlsx
+++ b/InputData/elec/DCpUC/Decommissioning Cost per Unit Cap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\DCpUC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64C09F4-3652-4E69-812F-4EC7CE2F3549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD7E634-93BC-45AD-B6F7-923947363AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>DCpUC Decommissioning Cost per Unit Capacity</t>
   </si>
@@ -220,6 +220,24 @@
   </si>
   <si>
     <t>hydrogen</t>
+  </si>
+  <si>
+    <t>For CCS plants, we adjust the costs based on the ratio of CCS equipped CAPEX vs. CAPEX for the non-CCS equipped equivalents</t>
+  </si>
+  <si>
+    <t>(see file elec/CCaMC).</t>
+  </si>
+  <si>
+    <t>CCS CAPEX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-CCS CAPEX </t>
+  </si>
+  <si>
+    <t>Decomissioning Cost Multiplier</t>
+  </si>
+  <si>
+    <t>We do the same for small modular reactors.</t>
   </si>
 </sst>
 </file>
@@ -585,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,6 +736,21 @@
       </c>
       <c r="B28" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -733,9 +766,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:AE42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:B42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -901,7 +936,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -909,7 +944,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -918,13 +953,1207 @@
         <v>556213.01775147929</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="6">
         <f>B18*About!A28</f>
         <v>653882.08703345177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>2021</v>
+      </c>
+      <c r="C22">
+        <v>2022</v>
+      </c>
+      <c r="D22">
+        <v>2023</v>
+      </c>
+      <c r="E22">
+        <v>2024</v>
+      </c>
+      <c r="F22">
+        <v>2025</v>
+      </c>
+      <c r="G22">
+        <v>2026</v>
+      </c>
+      <c r="H22">
+        <v>2027</v>
+      </c>
+      <c r="I22">
+        <v>2028</v>
+      </c>
+      <c r="J22">
+        <v>2029</v>
+      </c>
+      <c r="K22">
+        <v>2030</v>
+      </c>
+      <c r="L22">
+        <v>2031</v>
+      </c>
+      <c r="M22">
+        <v>2032</v>
+      </c>
+      <c r="N22">
+        <v>2033</v>
+      </c>
+      <c r="O22">
+        <v>2034</v>
+      </c>
+      <c r="P22">
+        <v>2035</v>
+      </c>
+      <c r="Q22">
+        <v>2036</v>
+      </c>
+      <c r="R22">
+        <v>2037</v>
+      </c>
+      <c r="S22">
+        <v>2038</v>
+      </c>
+      <c r="T22">
+        <v>2039</v>
+      </c>
+      <c r="U22">
+        <v>2040</v>
+      </c>
+      <c r="V22">
+        <v>2041</v>
+      </c>
+      <c r="W22">
+        <v>2042</v>
+      </c>
+      <c r="X22">
+        <v>2043</v>
+      </c>
+      <c r="Y22">
+        <v>2044</v>
+      </c>
+      <c r="Z22">
+        <v>2045</v>
+      </c>
+      <c r="AA22">
+        <v>2046</v>
+      </c>
+      <c r="AB22">
+        <v>2047</v>
+      </c>
+      <c r="AC22">
+        <v>2048</v>
+      </c>
+      <c r="AD22">
+        <v>2049</v>
+      </c>
+      <c r="AE22">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>2103947.1325892224</v>
+      </c>
+      <c r="C23">
+        <v>2103947.1325892224</v>
+      </c>
+      <c r="D23">
+        <v>2058678.3176273326</v>
+      </c>
+      <c r="E23">
+        <v>2013514.7789793089</v>
+      </c>
+      <c r="F23">
+        <v>1968456.5166451489</v>
+      </c>
+      <c r="G23">
+        <v>1923187.7016832591</v>
+      </c>
+      <c r="H23">
+        <v>1878024.1630352335</v>
+      </c>
+      <c r="I23">
+        <v>1832755.3480733442</v>
+      </c>
+      <c r="J23">
+        <v>1787591.8094253195</v>
+      </c>
+      <c r="K23">
+        <v>1742428.2707772935</v>
+      </c>
+      <c r="L23">
+        <v>1697264.7321292693</v>
+      </c>
+      <c r="M23">
+        <v>1651995.91716738</v>
+      </c>
+      <c r="N23">
+        <v>1606832.3785193549</v>
+      </c>
+      <c r="O23">
+        <v>1561668.8398713293</v>
+      </c>
+      <c r="P23">
+        <v>1516505.3012233055</v>
+      </c>
+      <c r="Q23">
+        <v>1496186.9726473875</v>
+      </c>
+      <c r="R23">
+        <v>1476079.1966991983</v>
+      </c>
+      <c r="S23">
+        <v>1455866.1444371459</v>
+      </c>
+      <c r="T23">
+        <v>1435653.0921750939</v>
+      </c>
+      <c r="U23">
+        <v>1415440.0399130401</v>
+      </c>
+      <c r="V23">
+        <v>1395226.9876509863</v>
+      </c>
+      <c r="W23">
+        <v>1375013.9353889339</v>
+      </c>
+      <c r="X23">
+        <v>1354800.883126881</v>
+      </c>
+      <c r="Y23">
+        <v>1334587.8308648276</v>
+      </c>
+      <c r="Z23">
+        <v>1314374.7786027743</v>
+      </c>
+      <c r="AA23">
+        <v>1294161.7263407223</v>
+      </c>
+      <c r="AB23">
+        <v>1273843.3977648029</v>
+      </c>
+      <c r="AC23">
+        <v>1253735.6218166156</v>
+      </c>
+      <c r="AD23">
+        <v>1233417.2932406971</v>
+      </c>
+      <c r="AE23">
+        <v>1213309.5172925084</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24">
+        <v>1088381.5096704282</v>
+      </c>
+      <c r="C24">
+        <v>1088381.5096704282</v>
+      </c>
+      <c r="D24">
+        <v>1059692.5494764193</v>
+      </c>
+      <c r="E24">
+        <v>1030908.9062454656</v>
+      </c>
+      <c r="F24">
+        <v>1002219.9460514563</v>
+      </c>
+      <c r="G24">
+        <v>973530.9858574461</v>
+      </c>
+      <c r="H24">
+        <v>944842.02566343674</v>
+      </c>
+      <c r="I24">
+        <v>916058.38243248337</v>
+      </c>
+      <c r="J24">
+        <v>887369.42223847343</v>
+      </c>
+      <c r="K24">
+        <v>858680.46204446396</v>
+      </c>
+      <c r="L24">
+        <v>829896.8188135107</v>
+      </c>
+      <c r="M24">
+        <v>801207.858619501</v>
+      </c>
+      <c r="N24">
+        <v>772518.89842549199</v>
+      </c>
+      <c r="O24">
+        <v>743829.93823148217</v>
+      </c>
+      <c r="P24">
+        <v>715046.29500052845</v>
+      </c>
+      <c r="Q24">
+        <v>703779.01360420149</v>
+      </c>
+      <c r="R24">
+        <v>692606.41524481808</v>
+      </c>
+      <c r="S24">
+        <v>681339.13384849124</v>
+      </c>
+      <c r="T24">
+        <v>670071.85245216393</v>
+      </c>
+      <c r="U24">
+        <v>658804.57105583663</v>
+      </c>
+      <c r="V24">
+        <v>647631.97269645345</v>
+      </c>
+      <c r="W24">
+        <v>636364.69130012603</v>
+      </c>
+      <c r="X24">
+        <v>625097.40990379918</v>
+      </c>
+      <c r="Y24">
+        <v>613924.81154441554</v>
+      </c>
+      <c r="Z24">
+        <v>602657.53014808858</v>
+      </c>
+      <c r="AA24">
+        <v>591390.24875176116</v>
+      </c>
+      <c r="AB24">
+        <v>580217.6503923781</v>
+      </c>
+      <c r="AC24">
+        <v>568950.36899605079</v>
+      </c>
+      <c r="AD24">
+        <v>557683.08759972372</v>
+      </c>
+      <c r="AE24">
+        <v>546510.48924034019</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>1289895.7980194129</v>
+      </c>
+      <c r="C25">
+        <v>1424324.1264074175</v>
+      </c>
+      <c r="D25">
+        <v>1558752.454795422</v>
+      </c>
+      <c r="E25">
+        <v>1693180.7831834266</v>
+      </c>
+      <c r="F25">
+        <v>1796492.5482441923</v>
+      </c>
+      <c r="G25">
+        <v>1852795.2520174449</v>
+      </c>
+      <c r="H25">
+        <v>1874191.2898811991</v>
+      </c>
+      <c r="I25">
+        <v>1881812.3784608822</v>
+      </c>
+      <c r="J25">
+        <v>1887554.6549820662</v>
+      </c>
+      <c r="K25">
+        <v>1892600.8229622045</v>
+      </c>
+      <c r="L25">
+        <v>1905769.0332217179</v>
+      </c>
+      <c r="M25">
+        <v>1916724.9766968857</v>
+      </c>
+      <c r="N25">
+        <v>1923267.4696774059</v>
+      </c>
+      <c r="O25">
+        <v>1930862.8540630611</v>
+      </c>
+      <c r="P25">
+        <v>1937772.6115127895</v>
+      </c>
+      <c r="Q25">
+        <v>1948062.5376181658</v>
+      </c>
+      <c r="R25">
+        <v>1958121.3905415633</v>
+      </c>
+      <c r="S25">
+        <v>1965944.3727370212</v>
+      </c>
+      <c r="T25">
+        <v>1977867.6285998137</v>
+      </c>
+      <c r="U25">
+        <v>1986058.7633075011</v>
+      </c>
+      <c r="V25">
+        <v>1991682.6657695849</v>
+      </c>
+      <c r="W25">
+        <v>2001284.5248759086</v>
+      </c>
+      <c r="X25">
+        <v>2007869.0972648514</v>
+      </c>
+      <c r="Y25">
+        <v>2016326.5933504989</v>
+      </c>
+      <c r="Z25">
+        <v>2026393.7738523479</v>
+      </c>
+      <c r="AA25">
+        <v>2035925.2315814244</v>
+      </c>
+      <c r="AB25">
+        <v>2044107.679105334</v>
+      </c>
+      <c r="AC25">
+        <v>2053831.5934090288</v>
+      </c>
+      <c r="AD25">
+        <v>2065027.9763754746</v>
+      </c>
+      <c r="AE25">
+        <v>2090069.7248419826</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <v>2438353.2875842112</v>
+      </c>
+      <c r="C26">
+        <v>2438353.2875842112</v>
+      </c>
+      <c r="D26">
+        <v>2385889.3439434203</v>
+      </c>
+      <c r="E26">
+        <v>2333547.4094738881</v>
+      </c>
+      <c r="F26">
+        <v>2281327.4841756118</v>
+      </c>
+      <c r="G26">
+        <v>2228863.5405348209</v>
+      </c>
+      <c r="H26">
+        <v>2176521.6060652863</v>
+      </c>
+      <c r="I26">
+        <v>2124057.6624244954</v>
+      </c>
+      <c r="J26">
+        <v>2071715.7279549628</v>
+      </c>
+      <c r="K26">
+        <v>2019373.7934854277</v>
+      </c>
+      <c r="L26">
+        <v>1967031.8590158951</v>
+      </c>
+      <c r="M26">
+        <v>1914567.9153751046</v>
+      </c>
+      <c r="N26">
+        <v>1862225.9809055701</v>
+      </c>
+      <c r="O26">
+        <v>1809884.0464360365</v>
+      </c>
+      <c r="P26">
+        <v>1757542.1119665033</v>
+      </c>
+      <c r="Q26">
+        <v>1733994.3419137769</v>
+      </c>
+      <c r="R26">
+        <v>1710690.5902035641</v>
+      </c>
+      <c r="S26">
+        <v>1687264.8293220946</v>
+      </c>
+      <c r="T26">
+        <v>1663839.0684406259</v>
+      </c>
+      <c r="U26">
+        <v>1640413.3075591563</v>
+      </c>
+      <c r="V26">
+        <v>1616987.5466776863</v>
+      </c>
+      <c r="W26">
+        <v>1593561.7857962172</v>
+      </c>
+      <c r="X26">
+        <v>1570136.0249147471</v>
+      </c>
+      <c r="Y26">
+        <v>1546710.2640332771</v>
+      </c>
+      <c r="Z26">
+        <v>1523284.5031518075</v>
+      </c>
+      <c r="AA26">
+        <v>1499858.7422703393</v>
+      </c>
+      <c r="AB26">
+        <v>1476310.9722176106</v>
+      </c>
+      <c r="AC26">
+        <v>1453007.2205074001</v>
+      </c>
+      <c r="AD26">
+        <v>1429459.4504546723</v>
+      </c>
+      <c r="AE26">
+        <v>1406155.6987444595</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="C27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="D27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="E27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="F27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="G27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="H27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="I27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="J27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="K27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="L27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="M27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="N27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="O27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="P27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="Q27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="R27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="S27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="T27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="U27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="V27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="W27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="X27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="Y27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="Z27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="AA27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="AB27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="AC27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="AD27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+      <c r="AE27" s="6">
+        <v>588408.96230039559</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>2021</v>
+      </c>
+      <c r="C30">
+        <v>2022</v>
+      </c>
+      <c r="D30">
+        <v>2023</v>
+      </c>
+      <c r="E30">
+        <v>2024</v>
+      </c>
+      <c r="F30">
+        <v>2025</v>
+      </c>
+      <c r="G30">
+        <v>2026</v>
+      </c>
+      <c r="H30">
+        <v>2027</v>
+      </c>
+      <c r="I30">
+        <v>2028</v>
+      </c>
+      <c r="J30">
+        <v>2029</v>
+      </c>
+      <c r="K30">
+        <v>2030</v>
+      </c>
+      <c r="L30">
+        <v>2031</v>
+      </c>
+      <c r="M30">
+        <v>2032</v>
+      </c>
+      <c r="N30">
+        <v>2033</v>
+      </c>
+      <c r="O30">
+        <v>2034</v>
+      </c>
+      <c r="P30">
+        <v>2035</v>
+      </c>
+      <c r="Q30">
+        <v>2036</v>
+      </c>
+      <c r="R30">
+        <v>2037</v>
+      </c>
+      <c r="S30">
+        <v>2038</v>
+      </c>
+      <c r="T30">
+        <v>2039</v>
+      </c>
+      <c r="U30">
+        <v>2040</v>
+      </c>
+      <c r="V30">
+        <v>2041</v>
+      </c>
+      <c r="W30">
+        <v>2042</v>
+      </c>
+      <c r="X30">
+        <v>2043</v>
+      </c>
+      <c r="Y30">
+        <v>2044</v>
+      </c>
+      <c r="Z30">
+        <v>2045</v>
+      </c>
+      <c r="AA30">
+        <v>2046</v>
+      </c>
+      <c r="AB30">
+        <v>2047</v>
+      </c>
+      <c r="AC30">
+        <v>2048</v>
+      </c>
+      <c r="AD30">
+        <v>2049</v>
+      </c>
+      <c r="AE30">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>3007428.4581774496</v>
+      </c>
+      <c r="C31">
+        <v>3007428.4581774496</v>
+      </c>
+      <c r="D31">
+        <v>2991110.6295283963</v>
+      </c>
+      <c r="E31">
+        <v>2974687.5245654779</v>
+      </c>
+      <c r="F31">
+        <v>2958264.4196025603</v>
+      </c>
+      <c r="G31">
+        <v>2941946.590953507</v>
+      </c>
+      <c r="H31">
+        <v>2925523.4859905886</v>
+      </c>
+      <c r="I31">
+        <v>2909205.6573415357</v>
+      </c>
+      <c r="J31">
+        <v>2892782.5523786172</v>
+      </c>
+      <c r="K31">
+        <v>2876464.7237295639</v>
+      </c>
+      <c r="L31">
+        <v>2860041.6187666459</v>
+      </c>
+      <c r="M31">
+        <v>2843723.7901175921</v>
+      </c>
+      <c r="N31">
+        <v>2827300.6851546741</v>
+      </c>
+      <c r="O31">
+        <v>2810982.8565056212</v>
+      </c>
+      <c r="P31">
+        <v>2794559.7515427028</v>
+      </c>
+      <c r="Q31">
+        <v>2767819.5678210286</v>
+      </c>
+      <c r="R31">
+        <v>2740974.1077854894</v>
+      </c>
+      <c r="S31">
+        <v>2714128.6477499502</v>
+      </c>
+      <c r="T31">
+        <v>2687388.4640282756</v>
+      </c>
+      <c r="U31">
+        <v>2660543.0039927363</v>
+      </c>
+      <c r="V31">
+        <v>2633802.8202710627</v>
+      </c>
+      <c r="W31">
+        <v>2606957.360235523</v>
+      </c>
+      <c r="X31">
+        <v>2580217.1765138488</v>
+      </c>
+      <c r="Y31">
+        <v>2553371.7164783091</v>
+      </c>
+      <c r="Z31">
+        <v>2526631.532756635</v>
+      </c>
+      <c r="AA31">
+        <v>2499786.0727210953</v>
+      </c>
+      <c r="AB31">
+        <v>2473045.8889994216</v>
+      </c>
+      <c r="AC31">
+        <v>2446200.4289638819</v>
+      </c>
+      <c r="AD31">
+        <v>2419460.2452422078</v>
+      </c>
+      <c r="AE31">
+        <v>2392614.7852066685</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32">
+        <v>1087150.6301901576</v>
+      </c>
+      <c r="C32">
+        <v>1087150.6301901576</v>
+      </c>
+      <c r="D32">
+        <v>1076735.4961263256</v>
+      </c>
+      <c r="E32">
+        <v>1066415.0450994375</v>
+      </c>
+      <c r="F32">
+        <v>1055999.9110356057</v>
+      </c>
+      <c r="G32">
+        <v>1045584.7769717741</v>
+      </c>
+      <c r="H32">
+        <v>1035169.6429079421</v>
+      </c>
+      <c r="I32">
+        <v>1024849.1918810543</v>
+      </c>
+      <c r="J32">
+        <v>1014434.0578172224</v>
+      </c>
+      <c r="K32">
+        <v>1004018.9237533906</v>
+      </c>
+      <c r="L32">
+        <v>993698.47272650246</v>
+      </c>
+      <c r="M32">
+        <v>983283.33866267081</v>
+      </c>
+      <c r="N32">
+        <v>972868.20459883893</v>
+      </c>
+      <c r="O32">
+        <v>962453.07053500693</v>
+      </c>
+      <c r="P32">
+        <v>952132.61950811907</v>
+      </c>
+      <c r="Q32">
+        <v>944273.92744177312</v>
+      </c>
+      <c r="R32">
+        <v>936415.23537542752</v>
+      </c>
+      <c r="S32">
+        <v>928651.22634602536</v>
+      </c>
+      <c r="T32">
+        <v>920792.53427967953</v>
+      </c>
+      <c r="U32">
+        <v>913028.5252502776</v>
+      </c>
+      <c r="V32">
+        <v>905169.83318393177</v>
+      </c>
+      <c r="W32">
+        <v>897311.14111758606</v>
+      </c>
+      <c r="X32">
+        <v>889547.13208818412</v>
+      </c>
+      <c r="Y32">
+        <v>881688.44002183829</v>
+      </c>
+      <c r="Z32">
+        <v>873829.74795549235</v>
+      </c>
+      <c r="AA32">
+        <v>866065.73892609053</v>
+      </c>
+      <c r="AB32">
+        <v>858207.04685974459</v>
+      </c>
+      <c r="AC32">
+        <v>850348.35479339876</v>
+      </c>
+      <c r="AD32">
+        <v>842584.34576399683</v>
+      </c>
+      <c r="AE32">
+        <v>834725.65369765111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>4567459.2942504622</v>
+      </c>
+      <c r="C33">
+        <v>4415131.4446385521</v>
+      </c>
+      <c r="D33">
+        <v>4262803.5950266421</v>
+      </c>
+      <c r="E33">
+        <v>4110475.745414732</v>
+      </c>
+      <c r="F33">
+        <v>3989264.4591300599</v>
+      </c>
+      <c r="G33">
+        <v>3915062.2341329018</v>
+      </c>
+      <c r="H33">
+        <v>3875766.6750452421</v>
+      </c>
+      <c r="I33">
+        <v>3850246.0652416525</v>
+      </c>
+      <c r="J33">
+        <v>3826604.267496563</v>
+      </c>
+      <c r="K33">
+        <v>3803658.5782925193</v>
+      </c>
+      <c r="L33">
+        <v>3774170.2163288565</v>
+      </c>
+      <c r="M33">
+        <v>3746894.1211495395</v>
+      </c>
+      <c r="N33">
+        <v>3724031.476464869</v>
+      </c>
+      <c r="O33">
+        <v>3700115.9403750645</v>
+      </c>
+      <c r="P33">
+        <v>3676886.0312211867</v>
+      </c>
+      <c r="Q33">
+        <v>3650275.9534116611</v>
+      </c>
+      <c r="R33">
+        <v>3623896.9487841143</v>
+      </c>
+      <c r="S33">
+        <v>3599753.8148845071</v>
+      </c>
+      <c r="T33">
+        <v>3571510.4073175653</v>
+      </c>
+      <c r="U33">
+        <v>3546999.1209057285</v>
+      </c>
+      <c r="V33">
+        <v>3525055.0667394954</v>
+      </c>
+      <c r="W33">
+        <v>3499133.0559290224</v>
+      </c>
+      <c r="X33">
+        <v>3476228.3318359302</v>
+      </c>
+      <c r="Y33">
+        <v>3451450.6840461334</v>
+      </c>
+      <c r="Z33">
+        <v>3425063.3518401352</v>
+      </c>
+      <c r="AA33">
+        <v>3399211.7424069084</v>
+      </c>
+      <c r="AB33">
+        <v>3374709.1431788495</v>
+      </c>
+      <c r="AC33">
+        <v>3348665.0771710053</v>
+      </c>
+      <c r="AD33">
+        <v>7950962.5122480858</v>
+      </c>
+      <c r="AE33">
+        <v>7911207.6996868448</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34">
+        <v>3485435.9953173972</v>
+      </c>
+      <c r="C34">
+        <v>3485435.9953173972</v>
+      </c>
+      <c r="D34">
+        <v>3466524.5737724607</v>
+      </c>
+      <c r="E34">
+        <v>3447491.1430562665</v>
+      </c>
+      <c r="F34">
+        <v>3428457.7123400732</v>
+      </c>
+      <c r="G34">
+        <v>3409546.2907951367</v>
+      </c>
+      <c r="H34">
+        <v>3390512.860078942</v>
+      </c>
+      <c r="I34">
+        <v>3371601.4385340065</v>
+      </c>
+      <c r="J34">
+        <v>3352568.0078178118</v>
+      </c>
+      <c r="K34">
+        <v>3333656.5862728753</v>
+      </c>
+      <c r="L34">
+        <v>3314623.1555566816</v>
+      </c>
+      <c r="M34">
+        <v>3295711.7340117446</v>
+      </c>
+      <c r="N34">
+        <v>3276678.3032955509</v>
+      </c>
+      <c r="O34">
+        <v>3257766.8817506148</v>
+      </c>
+      <c r="P34">
+        <v>3238733.4510344206</v>
+      </c>
+      <c r="Q34">
+        <v>3207743.1215349766</v>
+      </c>
+      <c r="R34">
+        <v>3176630.7828642749</v>
+      </c>
+      <c r="S34">
+        <v>3145518.4441935732</v>
+      </c>
+      <c r="T34">
+        <v>3114528.1146941292</v>
+      </c>
+      <c r="U34">
+        <v>3083415.7760234275</v>
+      </c>
+      <c r="V34">
+        <v>3052425.446523984</v>
+      </c>
+      <c r="W34">
+        <v>3021313.1078532818</v>
+      </c>
+      <c r="X34">
+        <v>2990322.7783538383</v>
+      </c>
+      <c r="Y34">
+        <v>2959210.4396831361</v>
+      </c>
+      <c r="Z34">
+        <v>2928220.1101836921</v>
+      </c>
+      <c r="AA34">
+        <v>2897107.7715129899</v>
+      </c>
+      <c r="AB34">
+        <v>2866117.4420135464</v>
+      </c>
+      <c r="AC34">
+        <v>2835005.1033428442</v>
+      </c>
+      <c r="AD34">
+        <v>2804014.7738434006</v>
+      </c>
+      <c r="AE34">
+        <v>2772902.4351726989</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35">
+        <v>7998667.6914128698</v>
+      </c>
+      <c r="C35">
+        <v>7732140.6127499426</v>
+      </c>
+      <c r="D35">
+        <v>7465613.5340870135</v>
+      </c>
+      <c r="E35">
+        <v>7199086.4554240862</v>
+      </c>
+      <c r="F35">
+        <v>6868265.0672371704</v>
+      </c>
+      <c r="G35">
+        <v>6741015.3154564975</v>
+      </c>
+      <c r="H35">
+        <v>6673383.0516755227</v>
+      </c>
+      <c r="I35">
+        <v>6629468.9953674376</v>
+      </c>
+      <c r="J35">
+        <v>6588789.5438430253</v>
+      </c>
+      <c r="K35">
+        <v>6549310.0088325609</v>
+      </c>
+      <c r="L35">
+        <v>6498563.3748371275</v>
+      </c>
+      <c r="M35">
+        <v>6451626.9149244726</v>
+      </c>
+      <c r="N35">
+        <v>6412930.1203607358</v>
+      </c>
+      <c r="O35">
+        <v>6371775.6102709025</v>
+      </c>
+      <c r="P35">
+        <v>6331801.8069032012</v>
+      </c>
+      <c r="Q35">
+        <v>6286007.299150575</v>
+      </c>
+      <c r="R35">
+        <v>6240610.8710301137</v>
+      </c>
+      <c r="S35">
+        <v>6199064.5876227496</v>
+      </c>
+      <c r="T35">
+        <v>6150456.5821100837</v>
+      </c>
+      <c r="U35">
+        <v>6108276.4110980993</v>
+      </c>
+      <c r="V35">
+        <v>6070517.1301646149</v>
+      </c>
+      <c r="W35">
+        <v>6025908.0192318503</v>
+      </c>
+      <c r="X35">
+        <v>5986493.7983129658</v>
+      </c>
+      <c r="Y35">
+        <v>5943855.2651717626</v>
+      </c>
+      <c r="Z35">
+        <v>5898443.8204206424</v>
+      </c>
+      <c r="AA35">
+        <v>5853955.9456378166</v>
+      </c>
+      <c r="AB35">
+        <v>5811790.1238826262</v>
+      </c>
+      <c r="AC35">
+        <v>5768517.8432327369</v>
+      </c>
+      <c r="AD35">
+        <v>6253823.2431127187</v>
+      </c>
+      <c r="AE35">
+        <v>6176247.4600298516</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <f>B23/SUM(B23,B31)</f>
+        <v>0.41162053056516718</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39">
+        <f>B24/SUM(B24,B32)</f>
+        <v>0.50028289158723938</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40">
+        <f>B25/SUM(B25,B33)</f>
+        <v>0.22021813219446548</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41">
+        <f>B26/SUM(B26,B34)</f>
+        <v>0.41162053056516718</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42">
+        <f>B27/SUM(B27,B35)</f>
+        <v>6.8522616721483784E-2</v>
       </c>
     </row>
   </sheetData>
@@ -940,7 +2169,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,8 +2344,8 @@
         <v>55</v>
       </c>
       <c r="B19" s="6">
-        <f>B2</f>
-        <v>111923.81055552546</v>
+        <f>B2*(1+Data!B38)</f>
+        <v>157993.94883926612</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1124,8 +2353,8 @@
         <v>56</v>
       </c>
       <c r="B20" s="6">
-        <f>B4</f>
-        <v>14349.206481477622</v>
+        <f>B4*(1+Data!B39)</f>
+        <v>21527.868992013606</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1133,8 +2362,8 @@
         <v>57</v>
       </c>
       <c r="B21" s="6">
-        <f>B10</f>
-        <v>111923.81055552546</v>
+        <f>B10*(1+Data!B40)</f>
+        <v>136571.46306415048</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1142,8 +2371,8 @@
         <v>58</v>
       </c>
       <c r="B22" s="6">
-        <f>B14</f>
-        <v>111923.81055552546</v>
+        <f>B14+(1*Data!B41)</f>
+        <v>111924.22217605602</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1151,8 +2380,8 @@
         <v>59</v>
       </c>
       <c r="B23" s="6">
-        <f>B5</f>
-        <v>740897.3613269612</v>
+        <f>B5*(1+Data!B42)</f>
+        <v>791665.58724712732</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>